<commit_message>
moved sort algorithms to it's own directory
</commit_message>
<xml_diff>
--- a/sortAlgorithms/SortAlgorithmsPerfComparision.xlsx
+++ b/sortAlgorithms/SortAlgorithmsPerfComparision.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kkchinta/Documents/YOU/mycpp_git/cpp-generic-pgms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kkchinta/Documents/YOU/mycpp_git/cpp-generic-pgms/sortAlgorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -376,7 +376,7 @@
               <a:ea typeface="Arial" charset="0"/>
               <a:cs typeface="Arial" charset="0"/>
             </a:rPr>
-            <a:t>Row 7 to 8 - The inpur data is randomly distributed between 0 and N integers.</a:t>
+            <a:t>Row 7 to 8 - The input data is randomly distributed between 0 and N integers.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>

</xml_diff>